<commit_message>
Sua he so luong, demo tinh luong
</commit_message>
<xml_diff>
--- a/Bug_ADMIN.xlsx
+++ b/Bug_ADMIN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoc\[DA]\Demo\Studies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D244414F-4B09-4C5B-9283-89D84B66AF3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6386A8-892E-4761-9BF5-5381DA591CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="6" xr2:uid="{4A134181-4941-4367-86B2-B3C7E633755F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="7" activeTab="7" xr2:uid="{4A134181-4941-4367-86B2-B3C7E633755F}"/>
   </bookViews>
   <sheets>
     <sheet name="Màn đăng nhập" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Danh sách môn học" sheetId="5" r:id="rId5"/>
     <sheet name="Danh sách lớp" sheetId="6" r:id="rId6"/>
     <sheet name="Cách tính lương" sheetId="7" r:id="rId7"/>
+    <sheet name="VD Cách tính lương và học phí" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Nền?????????????</t>
   </si>
@@ -48,9 +49,6 @@
     <t>Cái list ở dưới là cái gì thế? Thấy có giáo viên mà sao ở đây k có list</t>
   </si>
   <si>
-    <t>Hệ số lương trong khoảng 0.5 - 0.8 (&lt; 1) gì chứ, sao lại là 2 3 4 dk</t>
-  </si>
-  <si>
     <t>Chưa hiển thị list học sinh</t>
   </si>
   <si>
@@ -103,13 +101,61 @@
   </si>
   <si>
     <t>Như thế thì hệ số lương sẽ rơi vào khoảng từ 1 - 2 (VD 1.2 1.4 1.5 1.7 1.8)</t>
+  </si>
+  <si>
+    <t>Hệ số lương trong khoảng 1 - 1.8 gì chứ, sao lại là 2 3 4 dk</t>
+  </si>
+  <si>
+    <t>Vào từng ô xem công thức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Môn toán </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GV A </t>
+  </si>
+  <si>
+    <t>Hệ số lương</t>
+  </si>
+  <si>
+    <t>Học phí lớp do GV A dạy</t>
+  </si>
+  <si>
+    <t>Số buổi/lớp/tuần</t>
+  </si>
+  <si>
+    <t>Số hs/lớp</t>
+  </si>
+  <si>
+    <t>Tháng 5 có 4 tuần</t>
+  </si>
+  <si>
+    <t>=&gt;</t>
+  </si>
+  <si>
+    <t>Tổng số buổi trong tháng 5 của 1 lớp</t>
+  </si>
+  <si>
+    <t>Học phí 1 hs</t>
+  </si>
+  <si>
+    <t>Học phí 1 lớp</t>
+  </si>
+  <si>
+    <t>Lương</t>
+  </si>
+  <si>
+    <t>GV B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,13 +164,27 @@
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -139,8 +199,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -995,19 +1062,19 @@
   <dimension ref="A16:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1028,17 +1095,17 @@
   <sheetData>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1059,28 +1126,28 @@
   <sheetData>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="N28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1101,12 +1168,12 @@
   <sheetData>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1122,7 +1189,7 @@
   </sheetPr>
   <dimension ref="A21:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -1130,36 +1197,241 @@
   <sheetData>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="K28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25DD0961-9B8D-41A8-838A-FE6940570884}">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2">
+        <f>B2*B4</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2">
+        <f>B6*4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2">
+        <f>B5*D9</f>
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2">
+        <f>D10*B7</f>
+        <v>16000000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3">
+        <f>D11*70%</f>
+        <v>11200000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2">
+        <f>B2*B15</f>
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="2">
+        <f>B17*4</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="2">
+        <f>B16*D20</f>
+        <v>1440000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="2">
+        <f>D21*B18</f>
+        <v>28800000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="3">
+        <f>D22*70%</f>
+        <v>20160000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>